<commit_message>
Added server auto control
</commit_message>
<xml_diff>
--- a/Server/winners.xlsx
+++ b/Server/winners.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20404"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20405"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TLP-001\PycharmProjects\ShabatMadat\Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB20CA0-2513-456E-8512-96F38C92B8E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CD89A6-0F4B-4F43-9E2A-7B47DBF9A655}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>חותמת זמן</t>
   </si>
@@ -28,7 +28,16 @@
     <t>איזה זוג ניצח מביניכם?</t>
   </si>
   <si>
-    <t>המנצחים (יובל סמו, אלכס גרין)</t>
+    <t>הקבוצה של: אור, המפקד, רון</t>
+  </si>
+  <si>
+    <t>הקבוצה של: איי, עמרי</t>
+  </si>
+  <si>
+    <t>הקבוצה של: דור, הקשבי</t>
+  </si>
+  <si>
+    <t>הקבוצה של: לא נתמך עי גוגל, טון</t>
   </si>
 </sst>
 </file>
@@ -314,11 +323,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H102"/>
+  <dimension ref="A1:H106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -343,12 +352,8 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>45270.49900462963</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -357,8 +362,12 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="A3" s="2">
+        <v>45284.786620370367</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -367,8 +376,12 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+      <c r="A4" s="2">
+        <v>45284.786817129629</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -377,8 +390,12 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="A5" s="2">
+        <v>45284.786909722221</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -387,8 +404,12 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="A6" s="2">
+        <v>45284.78701388889</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1356,6 +1377,46 @@
       <c r="G102" s="1"/>
       <c r="H102" s="1"/>
     </row>
+    <row r="103" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+      <c r="C103" s="1"/>
+      <c r="D103" s="1"/>
+      <c r="E103" s="1"/>
+      <c r="F103" s="1"/>
+      <c r="G103" s="1"/>
+      <c r="H103" s="1"/>
+    </row>
+    <row r="104" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
+      <c r="D104" s="1"/>
+      <c r="E104" s="1"/>
+      <c r="F104" s="1"/>
+      <c r="G104" s="1"/>
+      <c r="H104" s="1"/>
+    </row>
+    <row r="105" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+      <c r="C105" s="1"/>
+      <c r="D105" s="1"/>
+      <c r="E105" s="1"/>
+      <c r="F105" s="1"/>
+      <c r="G105" s="1"/>
+      <c r="H105" s="1"/>
+    </row>
+    <row r="106" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
+      <c r="C106" s="1"/>
+      <c r="D106" s="1"/>
+      <c r="E106" s="1"/>
+      <c r="F106" s="1"/>
+      <c r="G106" s="1"/>
+      <c r="H106" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Committing index.html for Game {27637515}, Stage 1
</commit_message>
<xml_diff>
--- a/Server/winners.xlsx
+++ b/Server/winners.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TLP-001\PycharmProjects\ShabatMadat\Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CD89A6-0F4B-4F43-9E2A-7B47DBF9A655}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B68659-3946-4467-A060-28AA914EC3D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,16 +28,16 @@
     <t>איזה זוג ניצח מביניכם?</t>
   </si>
   <si>
-    <t>הקבוצה של: אור, המפקד, רון</t>
+    <t>הקבוצה של: טון, לא נתמך עי גוגל, המפקד</t>
   </si>
   <si>
-    <t>הקבוצה של: איי, עמרי</t>
+    <t>הקבוצה של: דור, אלכס</t>
   </si>
   <si>
-    <t>הקבוצה של: דור, הקשבי</t>
+    <t>הקבוצה של: איי, הקשבי</t>
   </si>
   <si>
-    <t>הקבוצה של: לא נתמך עי גוגל, טון</t>
+    <t>הקבוצה של: אריה, עמרי</t>
   </si>
 </sst>
 </file>
@@ -323,11 +323,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H106"/>
+  <dimension ref="A1:H110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -362,12 +362,8 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>45284.786620370367</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -376,12 +372,8 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>45284.786817129629</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -390,12 +382,8 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>45284.786909722221</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -404,12 +392,8 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>45284.78701388889</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -418,8 +402,12 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="2">
+        <v>45285.016736111109</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -428,8 +416,12 @@
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="2">
+        <v>45285.016840277778</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -438,8 +430,12 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="2">
+        <v>45285.016932870371</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -448,8 +444,12 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="2">
+        <v>45285.017025462963</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1417,6 +1417,46 @@
       <c r="G106" s="1"/>
       <c r="H106" s="1"/>
     </row>
+    <row r="107" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
+      <c r="D107" s="1"/>
+      <c r="E107" s="1"/>
+      <c r="F107" s="1"/>
+      <c r="G107" s="1"/>
+      <c r="H107" s="1"/>
+    </row>
+    <row r="108" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1"/>
+      <c r="E108" s="1"/>
+      <c r="F108" s="1"/>
+      <c r="G108" s="1"/>
+      <c r="H108" s="1"/>
+    </row>
+    <row r="109" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
+      <c r="C109" s="1"/>
+      <c r="D109" s="1"/>
+      <c r="E109" s="1"/>
+      <c r="F109" s="1"/>
+      <c r="G109" s="1"/>
+      <c r="H109" s="1"/>
+    </row>
+    <row r="110" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
+      <c r="C110" s="1"/>
+      <c r="D110" s="1"/>
+      <c r="E110" s="1"/>
+      <c r="F110" s="1"/>
+      <c r="G110" s="1"/>
+      <c r="H110" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Committing index.html for Game {63960141}, Stage 2
</commit_message>
<xml_diff>
--- a/Server/winners.xlsx
+++ b/Server/winners.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TLP-001\PycharmProjects\ShabatMadat\Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B68659-3946-4467-A060-28AA914EC3D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7CEED5-CFDC-4373-B974-A45DAC616F95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,16 +28,16 @@
     <t>איזה זוג ניצח מביניכם?</t>
   </si>
   <si>
-    <t>הקבוצה של: טון, לא נתמך עי גוגל, המפקד</t>
+    <t>הקבוצה של: אור, שרי</t>
   </si>
   <si>
-    <t>הקבוצה של: דור, אלכס</t>
+    <t>הקבוצה של: המפקד, הקשבי</t>
   </si>
   <si>
-    <t>הקבוצה של: איי, הקשבי</t>
+    <t>הקבוצה של: איי, עמרי</t>
   </si>
   <si>
-    <t>הקבוצה של: אריה, עמרי</t>
+    <t>הקבוצה של: דור, גור</t>
   </si>
 </sst>
 </file>
@@ -323,11 +323,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H110"/>
+  <dimension ref="A1:H114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -402,12 +402,8 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>45285.016736111109</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -416,12 +412,8 @@
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>45285.016840277778</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -430,12 +422,8 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>45285.016932870371</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -444,12 +432,8 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>45285.017025462963</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -458,8 +442,12 @@
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="A11" s="2">
+        <v>45285.022210648145</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -468,8 +456,12 @@
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="A12" s="2">
+        <v>45285.022337962961</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -478,8 +470,12 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="A13" s="2">
+        <v>45285.022418981483</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -488,8 +484,12 @@
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+      <c r="A14" s="2">
+        <v>45285.022499999999</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1457,6 +1457,46 @@
       <c r="G110" s="1"/>
       <c r="H110" s="1"/>
     </row>
+    <row r="111" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="1"/>
+      <c r="B111" s="1"/>
+      <c r="C111" s="1"/>
+      <c r="D111" s="1"/>
+      <c r="E111" s="1"/>
+      <c r="F111" s="1"/>
+      <c r="G111" s="1"/>
+      <c r="H111" s="1"/>
+    </row>
+    <row r="112" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+      <c r="C112" s="1"/>
+      <c r="D112" s="1"/>
+      <c r="E112" s="1"/>
+      <c r="F112" s="1"/>
+      <c r="G112" s="1"/>
+      <c r="H112" s="1"/>
+    </row>
+    <row r="113" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
+      <c r="C113" s="1"/>
+      <c r="D113" s="1"/>
+      <c r="E113" s="1"/>
+      <c r="F113" s="1"/>
+      <c r="G113" s="1"/>
+      <c r="H113" s="1"/>
+    </row>
+    <row r="114" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
+      <c r="C114" s="1"/>
+      <c r="D114" s="1"/>
+      <c r="E114" s="1"/>
+      <c r="F114" s="1"/>
+      <c r="G114" s="1"/>
+      <c r="H114" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Advanced the server a little bit more
</commit_message>
<xml_diff>
--- a/Server/winners.xlsx
+++ b/Server/winners.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TLP-001\PycharmProjects\ShabatMadat\Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7CEED5-CFDC-4373-B974-A45DAC616F95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B54E04-0999-49CC-98C5-79855ACD694F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,16 +28,16 @@
     <t>איזה זוג ניצח מביניכם?</t>
   </si>
   <si>
-    <t>הקבוצה של: אור, שרי</t>
+    <t>הקבוצה של: נועם, הקשבי, המפקד</t>
   </si>
   <si>
-    <t>הקבוצה של: המפקד, הקשבי</t>
+    <t>הקבוצה של: טון, אריה</t>
   </si>
   <si>
-    <t>הקבוצה של: איי, עמרי</t>
+    <t>הקבוצה של: אלכס, היייי</t>
   </si>
   <si>
-    <t>הקבוצה של: דור, גור</t>
+    <t>הקבוצה של: אור, שרי</t>
   </si>
 </sst>
 </file>
@@ -327,7 +327,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -351,9 +351,11 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+    <row r="2" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -362,8 +364,10 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -372,8 +376,10 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -382,8 +388,10 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -442,12 +450,8 @@
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>45285.022210648145</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -456,12 +460,8 @@
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>45285.022337962961</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="A12" s="2"/>
+      <c r="B12" s="3"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -470,12 +470,8 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
-        <v>45285.022418981483</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="A13" s="2"/>
+      <c r="B13" s="3"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -484,12 +480,8 @@
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>45285.022499999999</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="A14" s="2"/>
+      <c r="B14" s="3"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>

</xml_diff>